<commit_message>
fix same-date calculation for "Happy Birthday" screen.
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675" activeTab="3"/>
+    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>When were you born?</t>
-  </si>
-  <si>
-    <t>data('born') &amp;&amp; data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
   </si>
   <si>
     <t>Happy Birthday!</t>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t>table_id</t>
+  </si>
+  <si>
+    <t>data('born') &amp;&amp; data('born').getDate() === now().getDate() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -704,7 +704,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U154"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -941,10 +941,10 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -953,28 +953,28 @@
         <v>0</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>5</v>
@@ -998,7 +998,7 @@
         <v>11</v>
       </c>
       <c r="U1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
@@ -1007,21 +1007,21 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" t="s">
         <v>151</v>
-      </c>
-      <c r="I2" t="s">
-        <v>152</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="4" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1089,17 +1089,17 @@
     </row>
     <row r="9" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="I14" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" t="s">
@@ -1173,14 +1173,14 @@
     </row>
     <row r="15" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -1202,14 +1202,14 @@
     </row>
     <row r="18" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
@@ -1219,21 +1219,21 @@
     </row>
     <row r="20" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" t="s">
         <v>36</v>
       </c>
       <c r="H21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
@@ -1250,24 +1250,24 @@
     </row>
     <row r="23" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="27" spans="3:21" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1303,11 +1303,11 @@
       </c>
       <c r="F28" s="1"/>
       <c r="I28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U28" t="b">
         <v>1</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="29" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1324,34 +1324,34 @@
     </row>
     <row r="30" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1360,10 +1360,10 @@
     </row>
     <row r="33" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1376,17 +1376,17 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="36" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1411,32 +1411,32 @@
     </row>
     <row r="37" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -1447,23 +1447,23 @@
     </row>
     <row r="40" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E40" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="4"/>
@@ -1475,29 +1475,29 @@
     </row>
     <row r="42" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" t="s">
         <v>136</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -1507,25 +1507,25 @@
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="3:10" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J47" s="2"/>
     </row>
@@ -1535,23 +1535,23 @@
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J48" s="2"/>
     </row>
     <row r="49" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="51" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="52" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="1"/>
       <c r="I52" s="2"/>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="I53" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J53" s="2"/>
       <c r="U53" t="b">
@@ -1597,53 +1597,53 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" t="s">
+        <v>67</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" t="s">
+        <v>69</v>
+      </c>
+      <c r="R54" t="s">
         <v>70</v>
       </c>
-      <c r="R54" t="s">
+      <c r="S54" t="s">
         <v>71</v>
-      </c>
-      <c r="S54" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="55" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E55" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="J55" s="2"/>
     </row>
     <row r="56" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E56" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="J56" s="2"/>
     </row>
     <row r="57" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F57" s="1"/>
       <c r="I57" s="2"/>
@@ -1655,15 +1655,15 @@
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J58" s="2"/>
       <c r="N58" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U58" t="b">
         <v>1</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="59" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="60" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -1695,14 +1695,14 @@
     </row>
     <row r="61" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E61" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -1714,18 +1714,18 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" t="s">
+        <v>82</v>
+      </c>
+      <c r="O62" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="P62" s="1">
         <v>1</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="63" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="3:21" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1856,18 +1856,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1897,112 +1897,112 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2011,10 +2011,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
         <v>101</v>
-      </c>
-      <c r="C12" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2022,10 +2022,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
         <v>103</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2033,10 +2033,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2044,10 +2044,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2066,10 +2066,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2077,10 +2077,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
         <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2088,33 +2088,33 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
         <v>109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
         <v>111</v>
       </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2133,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2146,26 +2146,26 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1">
         <v>20130408</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix for insertion of default locale into list of locales and fix for example form translations list to reference english and hindi
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675" activeTab="1"/>
+    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -539,9 +539,6 @@
     <t>display.constraint_message.text</t>
   </si>
   <si>
-    <t>display.title.text</t>
-  </si>
-  <si>
     <t>string_token</t>
   </si>
   <si>
@@ -585,6 +582,9 @@
   </si>
   <si>
     <t>display.prompt</t>
+  </si>
+  <si>
+    <t>display.title.text.english</t>
   </si>
 </sst>
 </file>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V154"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1048,7 @@
         <v>151</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>143</v>
@@ -1096,7 +1096,7 @@
         <v>145</v>
       </c>
       <c r="J2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -1962,7 +1962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1975,24 +1975,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
         <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2315,16 +2315,16 @@
         <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
         <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -2351,29 +2351,29 @@
         <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" t="s">
         <v>162</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>163</v>
-      </c>
-      <c r="F5" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
         <v>165</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>166</v>
-      </c>
-      <c r="F6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Demonstrate setting a default value for a select-multiple list.
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675" activeTab="3"/>
+    <workbookView xWindow="1924" yWindow="6362" windowWidth="27295" windowHeight="14675" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="table_specific_translations" sheetId="5" r:id="rId2"/>
     <sheet name="calculates" sheetId="2" r:id="rId3"/>
     <sheet name="choices" sheetId="3" r:id="rId4"/>
-    <sheet name="settings" sheetId="4" r:id="rId5"/>
+    <sheet name="model" sheetId="6" r:id="rId5"/>
+    <sheet name="settings" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="173">
   <si>
     <t>type</t>
   </si>
@@ -585,6 +586,9 @@
   </si>
   <si>
     <t>display.title.text</t>
+  </si>
+  <si>
+    <t>default[0]</t>
   </si>
 </sst>
 </file>
@@ -998,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V154"/>
   <sheetViews>
-    <sheetView topLeftCell="C43" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2044,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2290,6 +2294,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Make super simple demo app
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -80,6 +80,9 @@
     <t xml:space="preserve">Enter your name</t>
   </si>
   <si>
+    <t xml:space="preserve">Name hint text!</t>
+  </si>
+  <si>
     <t xml:space="preserve">acknowledge</t>
   </si>
   <si>
@@ -197,7 +200,7 @@
     <t xml:space="preserve">Might be required</t>
   </si>
   <si>
-    <t xml:space="preserve">data('make_above_required') == 'yes'</t>
+    <t xml:space="preserve">data('make_above_required') == 'yes' || data('make_above_required') == null</t>
   </si>
   <si>
     <t xml:space="preserve">select_one</t>
@@ -290,49 +293,16 @@
     <t xml:space="preserve">openRowInitialElementKeyToValueMap</t>
   </si>
   <si>
-    <t xml:space="preserve">refrigerator_model_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refrigerator_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalog_id &gt;= ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['0']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'catalog_id&gt;='+opendatakit.encodeURIValue(0)</t>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"regions1-2.csv"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_.chain(context).pluck('regionLevel1').uniq().map(function(regionLevel1){ return {name:regionLevel1, label:regionLevel1, data_value:regionLevel1, display:{title: {text:regionLevel1}}}; }).value()</t>
   </si>
   <si>
     <t xml:space="preserve">{}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_facility_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin_region = ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[data('adminRegion')]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'facility_id&gt;='+opendatakit.encodeURIValue(0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"regions1-2.csv"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_.chain(context).pluck('regionLevel1').uniq().map(function(regionLevel1){ return {name:regionLevel1, label:regionLevel1, data_value:regionLevel1, display:{title: {text:regionLevel1}}}; }).value()</t>
   </si>
   <si>
     <t xml:space="preserve">_.map(context, function(place){ place.name = place.regionLevel2; place.label = place.regionLevel2; place.data_value = place.name; place.display = {title: {text:place.label}}; return place; })</t>
@@ -512,7 +482,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,10 +517,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -645,8 +611,8 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,35 +701,38 @@
       <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="L3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="4"/>
       <c r="N4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -781,61 +750,61 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3"/>
       <c r="J10" s="6"/>
@@ -851,16 +820,16 @@
     <row r="12" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J12" s="6"/>
       <c r="M12" s="0" t="n">
@@ -870,16 +839,16 @@
     <row r="13" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J13" s="6"/>
       <c r="M13" s="0" t="n">
@@ -892,33 +861,33 @@
         <v>16</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="D15" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J15" s="6"/>
       <c r="L15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3"/>
       <c r="J16" s="6"/>
@@ -933,24 +902,24 @@
         <v>16</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -958,39 +927,39 @@
         <v>16</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" s="3"/>
       <c r="J22" s="6"/>
@@ -1008,21 +977,21 @@
         <v>16</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1036,33 +1005,33 @@
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1114,10 +1083,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1125,24 +1094,24 @@
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1185,10 +1154,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1207,159 +1176,97 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="J2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="K2" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="4" t="s">
-        <v>99</v>
+      <c r="G3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="J3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>102</v>
+      <c r="H4" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1386,77 +1293,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="11" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="11" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="10" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="11" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D4" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1490,11 +1397,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>119</v>
+      <c r="A1" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -1502,23 +1409,23 @@
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170726</v>
@@ -1526,15 +1433,15 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add new stuff to xlsx
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -155,109 +155,157 @@
     <t xml:space="preserve">You can only type numbers in these two boxes</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">operation</t>
+  </si>
+  <si>
     <t xml:space="preserve">add_two</t>
   </si>
   <si>
-    <t xml:space="preserve">Second addition number</t>
+    <t xml:space="preserve">add_res</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eval(data('add_one') + data('operation') + data('add_two'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiply_res</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiply result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result of multiplying the result on the previous page by two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number(data('add_res')) * 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possibly_required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibly required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Might be required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('make_above_required') == 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yesno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make_above_required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make above required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select yes here to make the previous question required!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possibly_required_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibly required 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave this blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('make_prev_required') == 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make_prev_required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make previous page required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecting yes will make the prompt on the previous page required. You won’t be able to finalize until you go back. Also, the only allowed answer to this question is yes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only allowed answer is yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">+</t>
   </si>
   <si>
-    <t xml:space="preserve">add_res</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addition result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number(data('add_one')) + Number(data('add_two'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiply_res</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiply result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result of multiplying the two numbers on the previous page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number(data('add_one')) * Number(data('add_two'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possibly_required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibly required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Might be required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data('make_above_required') == 'yes'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yesno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make_above_required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make above required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select yes here to make the previous question required!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possibly_required_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibly required 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leave this blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data('make_prev_required') == 'yes'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make_prev_required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make previous page required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selecting yes will make the prompt on the previous page required. You won’t be able to finalize until you go back. Also, the only allowed answer to this question is yes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The only allowed answer is yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divided By</t>
   </si>
   <si>
     <t xml:space="preserve">query_name</t>
@@ -609,10 +657,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -839,218 +887,293 @@
     <row r="13" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="0" t="s">
         <v>45</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="M13" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="J14" s="6"/>
+      <c r="M14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="J15" s="6"/>
-      <c r="L15" s="0" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="0" t="s">
+      <c r="D16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="L16" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5"/>
+      <c r="B17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="D17" s="3"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="J22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D23" s="3"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="0" t="s">
+    <row r="24" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5"/>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5"/>
+      <c r="D25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="G25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5"/>
+      <c r="D26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="F26" s="0" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5"/>
       <c r="D27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5"/>
+      <c r="D28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="F28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5"/>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D31" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N27" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="O27" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="N34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1070,7 +1193,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1083,10 +1206,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1097,10 +1220,10 @@
         <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1108,16 +1231,57 @@
         <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1176,37 +1340,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,19 +1378,19 @@
         <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,19 +1398,19 @@
         <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,19 +1418,19 @@
         <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1300,70 +1464,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1398,10 +1562,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -1409,23 +1573,23 @@
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170726</v>
@@ -1433,15 +1597,15 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Fix mistake in xlsx
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -5024,7 +5024,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5186,7 +5186,7 @@
         <v>126</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Linked table prompts work
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,13 +15,17 @@
     <sheet name="media" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="calculates_demo" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="user_branch" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="hard_stuff" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="choices" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="queries" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="settings" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="properties" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="model" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="calculates" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="linked_table" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="household" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="members" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="education" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="hard_stuff" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="choices" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="queries" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="settings" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="properties" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="model" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="calculates" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="268">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -155,6 +159,12 @@
     <t xml:space="preserve">do section hard_stuff</t>
   </si>
   <si>
+    <t xml:space="preserve">selected(data('sections'), 'linked_table')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do section linked_table</t>
+  </si>
+  <si>
     <t xml:space="preserve">constraint</t>
   </si>
   <si>
@@ -395,15 +405,15 @@
     <t xml:space="preserve">Select where to go next</t>
   </si>
   <si>
+    <t xml:space="preserve">exit section</t>
+  </si>
+  <si>
     <t xml:space="preserve">some label 1</t>
   </si>
   <si>
     <t xml:space="preserve">You are at some label 1</t>
   </si>
   <si>
-    <t xml:space="preserve">exit section</t>
-  </si>
-  <si>
     <t xml:space="preserve">some label 2</t>
   </si>
   <si>
@@ -416,6 +426,114 @@
     <t xml:space="preserve">You are at some label 3</t>
   </si>
   <si>
+    <t xml:space="preserve">do section household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do section members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do section education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.button_label.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique barcode ID or locator designation for this household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('household_id') == null ? row_id == undefined ? '' : row_id : data('household_id')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row_id is formgen specific</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many rooms does the house contain?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the house have electricity?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the house have running water?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capture the household location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.new_instance_label.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Members Section:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section is used to gather information about all household members.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make a list of all individuals who normally live in this household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add House Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_linked_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who is the owner of the household?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">youngest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who are the two youngest members of the household?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hide_add_instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hide_delete_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section is used to gather education information on the relevant household members.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_members_education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questions are asked to members of the household who are at least 5 years old.</t>
+  </si>
+  <si>
     <t xml:space="preserve">possibly_required</t>
   </si>
   <si>
@@ -569,6 +687,9 @@
     <t xml:space="preserve">User branch</t>
   </si>
   <si>
+    <t xml:space="preserve">Household demo (embedded linked table)</t>
+  </si>
+  <si>
     <t xml:space="preserve">query_name</t>
   </si>
   <si>
@@ -627,6 +748,27 @@
   </si>
   <si>
     <t xml:space="preserve">context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_id = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ data('household_id') ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{household_id: data('household_id')}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_id = ? and age &gt;= ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ data('household_id'), '5' ]</t>
   </si>
   <si>
     <t xml:space="preserve">setting_name</t>
@@ -806,7 +948,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -833,6 +975,30 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -936,7 +1102,7 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,9 +1376,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="30" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1275,10 +1456,723 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="82.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1288,7 +2182,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="39.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="42.99"/>
@@ -1296,112 +2190,196 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>186</v>
+      <c r="A1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>188</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>191</v>
+        <v>229</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>230</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>193</v>
+        <v>229</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>232</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>195</v>
+        <v>233</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>234</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>197</v>
+        <v>236</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1435,11 +2413,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>198</v>
+      <c r="A1" s="16" t="s">
+        <v>244</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>199</v>
+        <v>245</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -1447,23 +2425,23 @@
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>201</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170726</v>
@@ -1471,15 +2449,15 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>205</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>206</v>
+        <v>252</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
@@ -1498,7 +2476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1511,77 +2489,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="11" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="11" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="17" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="17" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>199</v>
+      <c r="A1" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>214</v>
+      <c r="A2" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>216</v>
+      <c r="A3" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>218</v>
+      <c r="A4" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1595,7 +2573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1621,10 +2599,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>213</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1638,7 +2616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1656,7 +2634,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -1670,10 +2648,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>221</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1741,10 +2719,10 @@
         <v>12</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>13</v>
@@ -1772,7 +2750,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
@@ -1780,32 +2758,32 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +2825,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -1885,7 +2863,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1907,60 +2885,60 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,10 +3016,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P1" s="0" t="s">
         <v>13</v>
@@ -2062,16 +3040,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J3" s="6"/>
       <c r="M3" s="0" t="s">
@@ -2080,28 +3058,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J5" s="6"/>
       <c r="M5" s="0" t="s">
@@ -2110,16 +3088,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J6" s="6"/>
     </row>
@@ -2128,11 +3106,11 @@
         <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J7" s="6"/>
       <c r="L7" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,29 +3118,29 @@
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J8" s="6"/>
       <c r="L8" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J9" s="6"/>
       <c r="P9" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,16 +3157,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,10 +3174,10 @@
         <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4956,19 +5934,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4976,80 +5954,80 @@
         <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5057,36 +6035,36 @@
         <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,16 +6152,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5191,7 +6169,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -5202,16 +6180,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,10 +6226,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5261,7 +6239,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -5284,66 +6262,71 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>120</v>
+      <c r="B3" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>121</v>
+      <c r="A4" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>124</v>
+      <c r="A7" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="D8" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>126</v>
+      <c r="A10" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
         <v>122</v>
       </c>
     </row>
@@ -5363,186 +6346,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>15</v>
-      </c>
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="N13" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5560,308 +6424,148 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="I2" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D6" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>144</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add missing education form
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -687,7 +687,7 @@
     <t xml:space="preserve">User branch</t>
   </si>
   <si>
-    <t xml:space="preserve">Household demo (embedded linked table)</t>
+    <t xml:space="preserve">Household demo (embedded linked table, multiple forms per table id)</t>
   </si>
   <si>
     <t xml:space="preserve">query_name</t>
@@ -948,7 +948,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -979,14 +979,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1467,7 +1459,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1492,32 +1484,32 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1577,61 +1569,61 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12" t="n">
+      <c r="D3" s="8"/>
+      <c r="E3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1850,8 +1842,8 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2190,31 +2182,31 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>225</v>
       </c>
       <c r="J1" s="0" t="s">
@@ -2234,7 +2226,7 @@
       <c r="G2" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>230</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -2254,7 +2246,7 @@
       <c r="G3" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="13" t="s">
         <v>232</v>
       </c>
       <c r="J3" s="0" t="s">
@@ -2274,7 +2266,7 @@
       <c r="G4" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>234</v>
       </c>
       <c r="J4" s="0" t="s">
@@ -2311,22 +2303,22 @@
       <c r="B6" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2340,7 +2332,7 @@
       <c r="C7" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>237</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -2349,10 +2341,10 @@
       <c r="F7" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2363,10 +2355,10 @@
       <c r="B8" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>237</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -2375,10 +2367,10 @@
       <c r="F8" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2413,7 +2405,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>244</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2489,76 +2481,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="17" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="17" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="15" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="15" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="15" t="s">
         <v>264</v>
       </c>
     </row>
@@ -6228,7 +6220,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -6485,7 +6477,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="I2" s="9" t="n">
+      <c r="I2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6498,7 +6490,6 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
-      <c r="I3" s="9"/>
       <c r="J3" s="0" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
Update exampleForm.xlsx and example form's formDef.json
fixed typo "Handlesbars" to correct usage Handlebars
</commit_message>
<xml_diff>
--- a/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/app/config/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>